<commit_message>
Removed kids from non_work and add to working
</commit_message>
<xml_diff>
--- a/sir_od_matrix/data_ang/od_matrix_no_working.xlsx
+++ b/sir_od_matrix/data_ang/od_matrix_no_working.xlsx
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4417</v>
+        <v>2286</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>24241</v>
+        <v>10749</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>7270</v>
+        <v>3686</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>3098</v>
+        <v>1827</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>7926</v>
+        <v>4063</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1732,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>28173</v>
+        <v>14242</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>13387</v>
+        <v>6333</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>12410</v>
+        <v>5639</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>8701</v>
+        <v>4325</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>4468</v>
+        <v>1981</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>12493</v>
+        <v>6552</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>13433</v>
+        <v>6666</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -3090,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>73398</v>
+        <v>33567</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>8948</v>
+        <v>4862</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -3478,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>10582</v>
+        <v>5275</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -3672,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>13801</v>
+        <v>6831</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -3866,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>11041</v>
+        <v>5466</v>
       </c>
       <c r="S18">
         <v>0</v>
@@ -4060,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>11497</v>
+        <v>6026</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -4254,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>8182</v>
+        <v>4234</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -4448,7 +4448,7 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>84456</v>
+        <v>38641</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -4642,7 +4642,7 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>18753</v>
+        <v>8844</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -4836,7 +4836,7 @@
         <v>0</v>
       </c>
       <c r="W23">
-        <v>9175</v>
+        <v>4485</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -5030,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="X24">
-        <v>17181</v>
+        <v>8605</v>
       </c>
       <c r="Y24">
         <v>0</v>
@@ -5224,7 +5224,7 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <v>12574</v>
+        <v>5851</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -5418,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>11262</v>
+        <v>5451</v>
       </c>
       <c r="AA26">
         <v>0</v>
@@ -5612,7 +5612,7 @@
         <v>0</v>
       </c>
       <c r="AA27">
-        <v>10790</v>
+        <v>5397</v>
       </c>
       <c r="AB27">
         <v>0</v>
@@ -5806,7 +5806,7 @@
         <v>0</v>
       </c>
       <c r="AB28">
-        <v>5390</v>
+        <v>2770</v>
       </c>
       <c r="AC28">
         <v>0</v>
@@ -6000,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="AC29">
-        <v>6129</v>
+        <v>3219</v>
       </c>
       <c r="AD29">
         <v>0</v>
@@ -6194,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="AD30">
-        <v>13064</v>
+        <v>6989</v>
       </c>
       <c r="AE30">
         <v>0</v>
@@ -6388,7 +6388,7 @@
         <v>0</v>
       </c>
       <c r="AE31">
-        <v>7068</v>
+        <v>3820</v>
       </c>
       <c r="AF31">
         <v>0</v>
@@ -6582,7 +6582,7 @@
         <v>0</v>
       </c>
       <c r="AF32">
-        <v>36962</v>
+        <v>15701</v>
       </c>
       <c r="AG32">
         <v>0</v>
@@ -6776,7 +6776,7 @@
         <v>0</v>
       </c>
       <c r="AG33">
-        <v>18560</v>
+        <v>8996</v>
       </c>
       <c r="AH33">
         <v>0</v>
@@ -6970,7 +6970,7 @@
         <v>0</v>
       </c>
       <c r="AH34">
-        <v>6709</v>
+        <v>3409</v>
       </c>
       <c r="AI34">
         <v>0</v>
@@ -7164,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="AI35">
-        <v>9699</v>
+        <v>4875</v>
       </c>
       <c r="AJ35">
         <v>0</v>
@@ -7358,7 +7358,7 @@
         <v>0</v>
       </c>
       <c r="AJ36">
-        <v>6763</v>
+        <v>3326</v>
       </c>
       <c r="AK36">
         <v>0</v>
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="AK37">
-        <v>10041</v>
+        <v>5170</v>
       </c>
       <c r="AL37">
         <v>0</v>
@@ -7746,7 +7746,7 @@
         <v>0</v>
       </c>
       <c r="AL38">
-        <v>34291</v>
+        <v>16401</v>
       </c>
       <c r="AM38">
         <v>0</v>
@@ -7940,7 +7940,7 @@
         <v>0</v>
       </c>
       <c r="AM39">
-        <v>4582</v>
+        <v>2320</v>
       </c>
       <c r="AN39">
         <v>0</v>
@@ -8134,7 +8134,7 @@
         <v>0</v>
       </c>
       <c r="AN40">
-        <v>15821</v>
+        <v>7957</v>
       </c>
       <c r="AO40">
         <v>0</v>
@@ -8328,7 +8328,7 @@
         <v>0</v>
       </c>
       <c r="AO41">
-        <v>10842</v>
+        <v>5915</v>
       </c>
       <c r="AP41">
         <v>0</v>
@@ -8522,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="AP42">
-        <v>7875</v>
+        <v>3926</v>
       </c>
       <c r="AQ42">
         <v>0</v>
@@ -8716,7 +8716,7 @@
         <v>0</v>
       </c>
       <c r="AQ43">
-        <v>11781</v>
+        <v>6223</v>
       </c>
       <c r="AR43">
         <v>0</v>
@@ -8910,7 +8910,7 @@
         <v>0</v>
       </c>
       <c r="AR44">
-        <v>24088</v>
+        <v>12289</v>
       </c>
       <c r="AS44">
         <v>0</v>
@@ -9104,7 +9104,7 @@
         <v>0</v>
       </c>
       <c r="AS45">
-        <v>37801</v>
+        <v>18007</v>
       </c>
       <c r="AT45">
         <v>0</v>
@@ -9298,7 +9298,7 @@
         <v>0</v>
       </c>
       <c r="AT46">
-        <v>5416</v>
+        <v>2545</v>
       </c>
       <c r="AU46">
         <v>0</v>
@@ -9492,7 +9492,7 @@
         <v>0</v>
       </c>
       <c r="AU47">
-        <v>32522</v>
+        <v>16343</v>
       </c>
       <c r="AV47">
         <v>0</v>
@@ -9686,7 +9686,7 @@
         <v>0</v>
       </c>
       <c r="AV48">
-        <v>9056</v>
+        <v>5019</v>
       </c>
       <c r="AW48">
         <v>0</v>
@@ -9880,7 +9880,7 @@
         <v>0</v>
       </c>
       <c r="AW49">
-        <v>60058</v>
+        <v>27492</v>
       </c>
       <c r="AX49">
         <v>0</v>
@@ -10074,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="AX50">
-        <v>4955</v>
+        <v>2478</v>
       </c>
       <c r="AY50">
         <v>0</v>
@@ -10268,7 +10268,7 @@
         <v>0</v>
       </c>
       <c r="AY51">
-        <v>12903</v>
+        <v>6203</v>
       </c>
       <c r="AZ51">
         <v>0</v>
@@ -10462,7 +10462,7 @@
         <v>0</v>
       </c>
       <c r="AZ52">
-        <v>7769</v>
+        <v>3798</v>
       </c>
       <c r="BA52">
         <v>0</v>
@@ -10656,7 +10656,7 @@
         <v>0</v>
       </c>
       <c r="BA53">
-        <v>7779</v>
+        <v>3874</v>
       </c>
       <c r="BB53">
         <v>0</v>
@@ -10850,7 +10850,7 @@
         <v>0</v>
       </c>
       <c r="BB54">
-        <v>9953</v>
+        <v>5214</v>
       </c>
       <c r="BC54">
         <v>0</v>
@@ -11044,7 +11044,7 @@
         <v>0</v>
       </c>
       <c r="BC55">
-        <v>81895</v>
+        <v>36404</v>
       </c>
       <c r="BD55">
         <v>0</v>
@@ -11238,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="BD56">
-        <v>17925</v>
+        <v>8829</v>
       </c>
       <c r="BE56">
         <v>0</v>
@@ -11432,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="BE57">
-        <v>13677</v>
+        <v>7789</v>
       </c>
       <c r="BF57">
         <v>0</v>
@@ -11626,7 +11626,7 @@
         <v>0</v>
       </c>
       <c r="BF58">
-        <v>19195</v>
+        <v>9616</v>
       </c>
       <c r="BG58">
         <v>0</v>
@@ -11820,7 +11820,7 @@
         <v>0</v>
       </c>
       <c r="BG59">
-        <v>11574</v>
+        <v>5474</v>
       </c>
       <c r="BH59">
         <v>0</v>
@@ -12014,7 +12014,7 @@
         <v>0</v>
       </c>
       <c r="BH60">
-        <v>8080</v>
+        <v>4144</v>
       </c>
       <c r="BI60">
         <v>0</v>
@@ -12208,7 +12208,7 @@
         <v>0</v>
       </c>
       <c r="BI61">
-        <v>20296</v>
+        <v>10136</v>
       </c>
       <c r="BJ61">
         <v>0</v>
@@ -12402,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="BJ62">
-        <v>9589</v>
+        <v>5275</v>
       </c>
       <c r="BK62">
         <v>0</v>
@@ -12596,7 +12596,7 @@
         <v>0</v>
       </c>
       <c r="BK63">
-        <v>8808</v>
+        <v>4731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>